<commit_message>
fixed some problems with the lexer not excluding comments right this then found a issue with the parser that it was adding extra with newlines so i had to fix it so that if there is no statement expression then we are not extending the list
</commit_message>
<xml_diff>
--- a/tools/enum_creater.xlsx
+++ b/tools/enum_creater.xlsx
@@ -1,34 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathan_pc\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathan_pc\CLionProjects\IC10_Interpreter\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{824D27A4-8BB1-4EEB-8D2A-6DFC7D0536D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A548312E-C624-4C44-A5BA-9CA9F5D0C065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NEWDATA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Query - Table1" description="Connection to the 'Table1' query in the workbook." type="5" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Query - Table1" description="Connection to the 'Table1' query in the workbook." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=Table1;Extended Properties=&quot;&quot;" command="SELECT * FROM [Table1]"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="430">
   <si>
     <t>abs</t>
   </si>
@@ -1323,7 +1336,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1872,13 +1885,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D403" totalsRowShown="0">
-  <autoFilter ref="A1:D403"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D403" totalsRowShown="0">
+  <autoFilter ref="A1:D403" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="command"/>
-    <tableColumn id="2" name="token type"/>
-    <tableColumn id="3" name="op type"/>
-    <tableColumn id="4" name="enum rep" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="command"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="token type"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="op type"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="enum rep" dataDxfId="0">
       <calculatedColumnFormula>"{"""&amp;A2&amp;""","&amp;B2&amp;","&amp;C2&amp;"}"&amp;","</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2182,12 +2195,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H403"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2227,6 +2240,9 @@
         <f t="shared" ref="D2:D64" si="0">"{"""&amp;A2&amp;""","&amp;B2&amp;","&amp;C2&amp;"}"&amp;","</f>
         <v>{"abs",TT_MATH,UNOP},</v>
       </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
       <c r="G2" t="s">
         <v>2</v>
       </c>
@@ -2248,6 +2264,9 @@
         <f t="shared" si="0"/>
         <v>{"acos",TT_MATH,UNOP},</v>
       </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
       <c r="G3" t="s">
         <v>6</v>
       </c>
@@ -2269,6 +2288,9 @@
         <f t="shared" si="0"/>
         <v>{"add",TT_BINOP,BINOP},</v>
       </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
       <c r="G4" t="s">
         <v>16</v>
       </c>
@@ -2290,6 +2312,9 @@
         <f t="shared" si="0"/>
         <v>{"alias",TT_ALIAS,UNOP},</v>
       </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
       <c r="G5" t="s">
         <v>89</v>
       </c>
@@ -2311,6 +2336,9 @@
         <f t="shared" si="0"/>
         <v>{"and",TT_BITOP,BINOP},</v>
       </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
       <c r="G6" t="s">
         <v>91</v>
       </c>
@@ -2332,6 +2360,9 @@
         <f t="shared" si="0"/>
         <v>{"asin",TT_MATH,UNOP},</v>
       </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
       <c r="G7" t="s">
         <v>416</v>
       </c>
@@ -2353,6 +2384,9 @@
         <f t="shared" si="0"/>
         <v>{"atan",TT_MATH,UNOP},</v>
       </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
       <c r="G8" t="s">
         <v>417</v>
       </c>
@@ -2374,6 +2408,9 @@
         <f t="shared" si="0"/>
         <v>{"atan2",TT_MATH,BINOP},</v>
       </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
       <c r="G9" t="s">
         <v>418</v>
       </c>
@@ -2395,6 +2432,9 @@
         <f t="shared" si="0"/>
         <v>{"bap",TT_JUMP,TRIOP},</v>
       </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
       <c r="G10" t="s">
         <v>419</v>
       </c>
@@ -2416,8 +2456,8 @@
         <f t="shared" si="0"/>
         <v>{"bapal",TT_JUMP,TRIOP},</v>
       </c>
-      <c r="G11" t="s">
-        <v>416</v>
+      <c r="F11">
+        <v>9</v>
       </c>
       <c r="H11" t="s">
         <v>173</v>
@@ -2437,6 +2477,9 @@
         <f t="shared" si="0"/>
         <v>{"bapz",TT_JUMP,BINOP},</v>
       </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
       <c r="H12" t="s">
         <v>422</v>
       </c>
@@ -2455,6 +2498,9 @@
         <f t="shared" si="0"/>
         <v>{"bapzal",TT_JUMP,BINOP},</v>
       </c>
+      <c r="F13">
+        <v>11</v>
+      </c>
       <c r="H13" t="s">
         <v>54</v>
       </c>
@@ -2473,6 +2519,9 @@
         <f t="shared" si="0"/>
         <v>{"bdns",TT_JUMP,UNOP},</v>
       </c>
+      <c r="F14">
+        <v>12</v>
+      </c>
       <c r="H14" t="s">
         <v>423</v>
       </c>
@@ -2491,6 +2540,9 @@
         <f t="shared" si="0"/>
         <v>{"bdnsal",TT_JUMP,UNOP},</v>
       </c>
+      <c r="F15">
+        <v>13</v>
+      </c>
       <c r="H15" t="s">
         <v>424</v>
       </c>
@@ -2509,6 +2561,9 @@
         <f t="shared" si="0"/>
         <v>{"bdse",TT_JUMP,UNOP},</v>
       </c>
+      <c r="F16">
+        <v>14</v>
+      </c>
       <c r="H16" t="s">
         <v>425</v>
       </c>
@@ -2527,6 +2582,9 @@
         <f t="shared" si="0"/>
         <v>{"bdseal",TT_JUMP,UNOP},</v>
       </c>
+      <c r="F17">
+        <v>15</v>
+      </c>
       <c r="H17" t="s">
         <v>154</v>
       </c>
@@ -2545,6 +2603,9 @@
         <f t="shared" si="0"/>
         <v>{"beq",TT_JUMP,BINOP},</v>
       </c>
+      <c r="F18">
+        <v>16</v>
+      </c>
       <c r="H18" t="s">
         <v>76</v>
       </c>
@@ -2563,6 +2624,9 @@
         <f t="shared" si="0"/>
         <v>{"beqal",TT_JUMP,BINOP},</v>
       </c>
+      <c r="F19">
+        <v>17</v>
+      </c>
       <c r="H19" t="s">
         <v>8</v>
       </c>
@@ -2581,6 +2645,9 @@
         <f t="shared" si="0"/>
         <v>{"beqz",TT_JUMP,UNOP},</v>
       </c>
+      <c r="F20">
+        <v>18</v>
+      </c>
       <c r="H20" t="s">
         <v>1</v>
       </c>
@@ -2599,6 +2666,9 @@
         <f t="shared" si="0"/>
         <v>{"beqzal",TT_JUMP,UNOP},</v>
       </c>
+      <c r="F21">
+        <v>19</v>
+      </c>
       <c r="H21" t="s">
         <v>112</v>
       </c>
@@ -2617,6 +2687,9 @@
         <f t="shared" si="0"/>
         <v>{"bge",TT_JUMP,BINOP},</v>
       </c>
+      <c r="F22">
+        <v>20</v>
+      </c>
       <c r="H22" t="s">
         <v>86</v>
       </c>
@@ -2635,6 +2708,9 @@
         <f t="shared" si="0"/>
         <v>{"bgeal",TT_JUMP,BINOP},</v>
       </c>
+      <c r="F23">
+        <v>21</v>
+      </c>
       <c r="H23" t="s">
         <v>181</v>
       </c>
@@ -2653,6 +2729,9 @@
         <f t="shared" si="0"/>
         <v>{"bgez",TT_JUMP,UNOP},</v>
       </c>
+      <c r="F24">
+        <v>22</v>
+      </c>
       <c r="H24" t="s">
         <v>106</v>
       </c>
@@ -2671,6 +2750,9 @@
         <f t="shared" si="0"/>
         <v>{"bgezal",TT_JUMP,UNOP},</v>
       </c>
+      <c r="F25">
+        <v>23</v>
+      </c>
       <c r="H25" t="s">
         <v>133</v>
       </c>
@@ -2689,6 +2771,9 @@
         <f t="shared" si="0"/>
         <v>{"bgt",TT_JUMP,BINOP},</v>
       </c>
+      <c r="F26">
+        <v>24</v>
+      </c>
       <c r="H26" t="s">
         <v>81</v>
       </c>
@@ -2707,6 +2792,9 @@
         <f t="shared" si="0"/>
         <v>{"bgtal",TT_JUMP,BINOP},</v>
       </c>
+      <c r="F27">
+        <v>25</v>
+      </c>
       <c r="H27" t="s">
         <v>410</v>
       </c>
@@ -8077,7 +8165,7 @@
         <v>419</v>
       </c>
       <c r="D385" t="str">
-        <f t="shared" ref="D385:D448" si="6">"{"""&amp;A385&amp;""","&amp;B385&amp;","&amp;C385&amp;"}"&amp;","</f>
+        <f t="shared" ref="D385:D403" si="6">"{"""&amp;A385&amp;""","&amp;B385&amp;","&amp;C385&amp;"}"&amp;","</f>
         <v>{"ratioliquidcarbondioxideoutput",TT_DPARA,TNULL},</v>
       </c>
     </row>
@@ -8354,10 +8442,10 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B403">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B403" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$H$2:$H$27</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C403">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C403" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>$G$2:$G$11</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
got first exicution command done
</commit_message>
<xml_diff>
--- a/tools/enum_creater.xlsx
+++ b/tools/enum_creater.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathan_pc\CLionProjects\IC10_Interpreter\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7AE31E-FDDA-403F-A130-EB566034E27D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAB5AB1-EF7F-48C7-B39D-604FD4B03240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NEWDATA" sheetId="1" r:id="rId1"/>
@@ -2211,8 +2211,8 @@
   <dimension ref="A1:I403"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D100" sqref="D100"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2331,18 +2331,18 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>431</v>
+        <v>8</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v>ALIAS</v>
+        <v>CNULL</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="1"/>
-        <v>{"alias",TT_CMD,UNOP,ALIAS},</v>
+        <v>{"alias",TT_ALIAS,UNOP,CNULL},</v>
       </c>
       <c r="G5">
         <v>3</v>
@@ -3687,18 +3687,18 @@
         <v>75</v>
       </c>
       <c r="B68" t="s">
-        <v>431</v>
+        <v>76</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="2"/>
-        <v>DEFINE</v>
+        <v>CNULL</v>
       </c>
       <c r="D68" t="s">
         <v>2</v>
       </c>
       <c r="E68" t="str">
-        <f t="shared" si="3"/>
-        <v>{"define",TT_CMD,UNOP,DEFINE},</v>
+        <f>"{"""&amp;A68&amp;""","&amp;B68&amp;","&amp;D68&amp;","&amp;C68&amp;"}"&amp;","</f>
+        <v>{"define",TT_DEFINE,UNOP,CNULL},</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -9732,14 +9732,14 @@
         <v>207</v>
       </c>
       <c r="C386" t="str">
-        <f t="shared" ref="C386:C449" si="12">IF(B386=$I$28,UPPER(A386),"CNULL")</f>
+        <f t="shared" ref="C386:C403" si="12">IF(B386=$I$28,UPPER(A386),"CNULL")</f>
         <v>CNULL</v>
       </c>
       <c r="D386" t="s">
         <v>419</v>
       </c>
       <c r="E386" t="str">
-        <f t="shared" ref="E386:E449" si="13">"{"""&amp;A386&amp;""","&amp;B386&amp;","&amp;D386&amp;","&amp;C386&amp;"}"&amp;","</f>
+        <f t="shared" ref="E386:E403" si="13">"{"""&amp;A386&amp;""","&amp;B386&amp;","&amp;D386&amp;","&amp;C386&amp;"}"&amp;","</f>
         <v>{"ratioliquidcarbondioxideoutput2",TT_DPARA,TNULL,CNULL},</v>
       </c>
     </row>

</xml_diff>

<commit_message>
most juming code is done finficed load now working on batch load
</commit_message>
<xml_diff>
--- a/tools/enum_creater.xlsx
+++ b/tools/enum_creater.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathan_pc\CLionProjects\IC10_Interpreter\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAB5AB1-EF7F-48C7-B39D-604FD4B03240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEE1DD3-B9B8-437A-BAB0-5B6298D8332B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2211,8 +2211,8 @@
   <dimension ref="A1:I403"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3941,11 +3941,11 @@
         <v>LOG</v>
       </c>
       <c r="D81" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E81" t="str">
         <f t="shared" si="3"/>
-        <v>{"log",TT_CMD,BINOP,LOG},</v>
+        <v>{"log",TT_CMD,UNOP,LOG},</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>